<commit_message>
import excel dataset mostly done
</commit_message>
<xml_diff>
--- a/src/test/resources/excelImport/minimalCaseNoMeasurementMoment.xlsx
+++ b/src/test/resources/excelImport/minimalCaseNoMeasurementMoment.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Study data" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="R1C1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -211,13 +211,13 @@
   </sheetPr>
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -246,11 +246,15 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -334,7 +338,7 @@
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:P1"/>
-    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M2:R2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" location="/users/1/datasets/ea775979-56f1-406e-9393-8faef7a2e630/versions/a306f265-4a93-4981-98d3-bb34e76ee885/studies/46813d09-2b71-4315-9ef6-11c4905e58d3%23design" display="http://localhost:8090/#/users/1/datasets/ea775979-56f1-406e-9393-8faef7a2e630/versions/a306f265-4a93-4981-98d3-bb34e76ee885/studies/46813d09-2b71-4315-9ef6-11c4905e58d3#design"/>

</xml_diff>